<commit_message>
Corrected ROR of institute of plasma physic (CAS)
</commit_message>
<xml_diff>
--- a/nr_vocabularies/fixtures/institutions.xlsx
+++ b/nr_vocabularies/fixtures/institutions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\metadatové modely\nr-github\nr-vocabularies\nr_vocabularies\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849CE1F0-111B-453D-9342-2C7B8D1DE11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357A4429-9C2E-4CAD-9967-7285B561411D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1569">
   <si>
     <t>code</t>
   </si>
@@ -4724,6 +4724,9 @@
   </si>
   <si>
     <t>deprecated</t>
+  </si>
+  <si>
+    <t>https://ror.org/01h494015</t>
   </si>
 </sst>
 </file>
@@ -4754,7 +4757,8 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4767,7 +4771,8 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4780,12 +4785,14 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4848,7 +4855,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4875,6 +4882,7 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -5153,8 +5161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1046981"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A147" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -9839,8 +9847,8 @@
       <c r="F144" s="9" t="s">
         <v>888</v>
       </c>
-      <c r="G144" s="9" t="s">
-        <v>883</v>
+      <c r="G144" s="16" t="s">
+        <v>1568</v>
       </c>
       <c r="H144" s="9" t="s">
         <v>889</v>
@@ -13672,7 +13680,7 @@
     </row>
     <row r="1046981" ht="12.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B6 B173:B174 B8:B64 B66:B171">
+  <conditionalFormatting sqref="B6 B8:B64 B66:B171 B173:B174">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Fakulta">
       <formula>NOT(ISERROR(SEARCH("Fakulta",B6)))</formula>
     </cfRule>
@@ -13700,6 +13708,7 @@
     <hyperlink ref="G197" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="H198" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="G199" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G144" r:id="rId23" xr:uid="{A67E16C5-3766-470E-B148-1C19C0B70392}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.51180555555555596"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Deleted ROR Institute of Hydrobiology(CAS)
</commit_message>
<xml_diff>
--- a/nr_vocabularies/fixtures/institutions.xlsx
+++ b/nr_vocabularies/fixtures/institutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\metadatové modely\nr-github\nr-vocabularies\nr_vocabularies\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357A4429-9C2E-4CAD-9967-7285B561411D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA25D8EB-071D-4D59-B934-D5F431570F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33345" yWindow="1785" windowWidth="21600" windowHeight="11265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slovník" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="1569">
   <si>
     <t>code</t>
   </si>
@@ -5162,7 +5162,7 @@
   <dimension ref="A1:P1046981"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G144" sqref="G144"/>
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -9175,9 +9175,7 @@
       <c r="F123" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="G123" s="9" t="s">
-        <v>684</v>
-      </c>
+      <c r="G123" s="9"/>
       <c r="H123" s="9" t="s">
         <v>766</v>
       </c>

</xml_diff>